<commit_message>
Gắn giao diện BNS và BDT
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/notification.xlsx
+++ b/Hethongquanlylab/wwwroot/data/notification.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -55,32 +55,27 @@
     <t>date</t>
   </si>
   <si>
+    <t>link</t>
+  </si>
+  <si>
     <t>Thông báo lịch họp dự án</t>
   </si>
   <si>
-    <t>Thông báo lịch làm việc 1-1</t>
-  </si>
-  <si>
-    <t>Thông báo đến dọn xưởng</t>
+    <t>Ban Nhân sự</t>
   </si>
   <si>
     <t>Thông báo tuyển dụng</t>
   </si>
   <si>
     <t>Ban Đào tạo</t>
-  </si>
-  <si>
-    <t>Ban Nhân sự</t>
-  </si>
-  <si>
-    <t>link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,11 +102,11 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257A422D-728B-44C1-B79B-EDEC61D007EF}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
@@ -436,125 +431,80 @@
   <cols>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0">
         <v>123321</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>123121</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="F2" s="1">
         <v>44690</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>12232</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>123123</v>
-      </c>
-      <c r="D3">
-        <v>3123</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="3">
+      <c r="A3" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0">
+        <v>132213</v>
+      </c>
+      <c r="D3" s="0">
+        <v>1231</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="1">
-        <v>44691</v>
-      </c>
-      <c r="G3">
-        <v>123213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>12312321</v>
-      </c>
-      <c r="D4">
-        <v>1231</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44692</v>
-      </c>
-      <c r="G4">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>132213</v>
-      </c>
-      <c r="D5">
-        <v>1231</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
         <v>44693</v>
       </c>
-      <c r="G5">
+      <c r="G3" s="0">
         <v>31232</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Chức năng Quy trình BNS + Function ExportTOExcel + MemberDetail + News
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/notification.xlsx
+++ b/Hethongquanlylab/wwwroot/data/notification.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4C88CF-78F1-4062-8D47-5FDC899869FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64266AC-2452-4DAD-B798-410A1B2C3DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="1110" windowWidth="21600" windowHeight="11295" xr2:uid="{0412304E-49F4-4854-A760-C021CC64E80A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{0412304E-49F4-4854-A760-C021CC64E80A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,8 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,11 +101,11 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="14" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,87 +423,74 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" bestFit="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>123321</v>
       </c>
-      <c r="D2" s="0">
-        <v>123121</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="1">
         <v>44690</v>
       </c>
-      <c r="G2" s="0">
-        <v>12232</v>
-      </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>132213</v>
       </c>
-      <c r="D3" s="0">
-        <v>1231</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="1">
         <v>44693</v>
-      </c>
-      <c r="G3" s="0">
-        <v>31232</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ghép chức năng và giao diện cho phần thông báo, quy trình, ban đào tạo
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/notification.xlsx
+++ b/Hethongquanlylab/wwwroot/data/notification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64266AC-2452-4DAD-B798-410A1B2C3DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C674A61-0615-4C7C-8A21-F9D55B23981F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{0412304E-49F4-4854-A760-C021CC64E80A}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8928" xr2:uid="{0412304E-49F4-4854-A760-C021CC64E80A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -68,6 +68,21 @@
   </si>
   <si>
     <t>Ban Đào tạo</t>
+  </si>
+  <si>
+    <t>rjqwehrew</t>
+  </si>
+  <si>
+    <t>Đề án cuộc thi NCKH</t>
+  </si>
+  <si>
+    <t>Đề án cuộc thi</t>
+  </si>
+  <si>
+    <t>fadfaf</t>
+  </si>
+  <si>
+    <t>BanDaoTao</t>
   </si>
 </sst>
 </file>
@@ -420,20 +435,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257A422D-728B-44C1-B79B-EDEC61D007EF}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
-    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="2" max="2" width="31.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -466,14 +482,20 @@
       <c r="C2">
         <v>123321</v>
       </c>
+      <c r="D2">
+        <v>1234</v>
+      </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="1">
         <v>44690</v>
       </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -483,11 +505,40 @@
       <c r="C3">
         <v>132213</v>
       </c>
+      <c r="D3">
+        <v>1234</v>
+      </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="1">
-        <v>44693</v>
+        <v>44691</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44692</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Paging trang tin tức
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/notification.xlsx
+++ b/Hethongquanlylab/wwwroot/data/notification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C674A61-0615-4C7C-8A21-F9D55B23981F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3071E2D2-E676-4F88-BF7C-D2EB78BFDA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8928" xr2:uid="{0412304E-49F4-4854-A760-C021CC64E80A}"/>
   </bookViews>
@@ -64,13 +64,13 @@
     <t>Ban Nhân sự</t>
   </si>
   <si>
+    <t>rjqwehrew</t>
+  </si>
+  <si>
     <t>Thông báo tuyển dụng</t>
   </si>
   <si>
     <t>Ban Đào tạo</t>
-  </si>
-  <si>
-    <t>rjqwehrew</t>
   </si>
   <si>
     <t>Đề án cuộc thi NCKH</t>
@@ -438,13 +438,14 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="31.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.109375" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
@@ -492,7 +493,7 @@
         <v>44690</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -500,7 +501,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>132213</v>
@@ -509,13 +510,13 @@
         <v>1234</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1">
         <v>44691</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -538,7 +539,7 @@
         <v>44692</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoàn thành cơ bản chức năng ban đào tạo
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/notification.xlsx
+++ b/Hethongquanlylab/wwwroot/data/notification.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3071E2D2-E676-4F88-BF7C-D2EB78BFDA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7765BEF5-96E8-4665-80FB-EA85C1C30D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8928" xr2:uid="{0412304E-49F4-4854-A760-C021CC64E80A}"/>
+    <workbookView xWindow="3924" yWindow="3312" windowWidth="16536" windowHeight="8928" xr2:uid="{0412304E-49F4-4854-A760-C021CC64E80A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -67,29 +67,27 @@
     <t>rjqwehrew</t>
   </si>
   <si>
-    <t>Thông báo tuyển dụng</t>
+    <t>Thông báo họp định kỳ Ban Đào tạo</t>
+  </si>
+  <si>
+    <t>&lt;p style="text-align: center;"&gt;&lt;span style="color: rgb(255, 0, 0);"&gt;Thông báo họp định kì ban Đào tạo&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>Ban Đào tạo</t>
   </si>
   <si>
-    <t>Đề án cuộc thi NCKH</t>
-  </si>
-  <si>
-    <t>Đề án cuộc thi</t>
-  </si>
-  <si>
-    <t>fadfaf</t>
-  </si>
-  <si>
-    <t>BanDaoTao</t>
+    <t>11/09/2022 09:15</t>
+  </si>
+  <si>
+    <t>fdajhfjdashfd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,11 +114,11 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,114 +433,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257A422D-728B-44C1-B79B-EDEC61D007EF}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="31.21875" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.109375" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>123321</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>1234</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="1">
         <v>44690</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3">
+      <c r="A3" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>132213</v>
-      </c>
-      <c r="D3">
-        <v>1234</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
-        <v>44691</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G3" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44692</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hoàn thiện giao diện đào tạo
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/notification.xlsx
+++ b/Hethongquanlylab/wwwroot/data/notification.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>dfdaffdaff</t>
+  </si>
+  <si>
+    <t>Thông báo qua xưởng làm</t>
+  </si>
+  <si>
+    <t>&lt;p style="text-align: center;"&gt;&lt;span style="color: rgb(255, 0, 0);"&gt;Yêu cầu 100% qua xưởng&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>14/09/2022 04:21</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/u/0/my-drive</t>
   </si>
 </sst>
 </file>
@@ -460,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257A422D-728B-44C1-B79B-EDEC61D007EF}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -581,6 +593,26 @@
         <v>23</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Sửa các lỗi nhỏ lẻ
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/notification.xlsx
+++ b/Hethongquanlylab/wwwroot/data/notification.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>https://us06web.zoom.us/postattendee?mn=bmYlpIgEcR-bI-lM1s-fjt1LNaCh6M98wrRh.9veeSYB9uE4OLuCg</t>
+  </si>
+  <si>
+    <t>Thông báo 1</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;123&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>19/09/2022 12:28</t>
   </si>
 </sst>
 </file>
@@ -502,7 +511,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257A422D-728B-44C1-B79B-EDEC61D007EF}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -696,6 +705,26 @@
         <v>37</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>